<commit_message>
Documentación variables y corrección i_star
</commit_message>
<xml_diff>
--- a/data/raw/2024-02/3 i star/i_star.xlsx
+++ b/data/raw/2024-02/3 i star/i_star.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGOR\Documents\SVAR50_APP\SVAR504B_APP\data\raw\2023-11\3 i star\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGOR\Documents\SVAR50_APP\SVAR504B_APP\data\raw\2024-02\3 i star\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E17D0525-4CF7-4E2A-AA9E-B87E200DA170}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA034C2-F7B4-4DFA-A5D4-3F5AD071861A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{DA6C5B1A-2C98-4ADC-B786-19A4A0D2B59C}"/>
   </bookViews>
@@ -908,6 +908,2519 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$277</c:f>
+              <c:strCache>
+                <c:ptCount val="276"/>
+                <c:pt idx="0">
+                  <c:v>2001M01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001M02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2001M03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2001M04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2001M05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2001M06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001M07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2001M08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2001M09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2001M10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2001M11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001M12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002M01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2002M02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2002M03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2002M04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2002M05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2002M06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2002M07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2002M08</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2002M09</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2002M10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2002M11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2002M12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2003M01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2003M02</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2003M03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2003M04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2003M05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2003M06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2003M07</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2003M08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2003M09</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2003M10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2003M11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2003M12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2004M01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2004M02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2004M03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2004M04</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2004M05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2004M06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2004M07</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2004M08</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2004M09</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2004M10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2004M11</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2004M12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2005M01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2005M02</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2005M03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2005M04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2005M05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2005M06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2005M07</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2005M08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2005M09</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2005M10</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2005M11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2005M12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2006M01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2006M02</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2006M03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2006M04</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2006M05</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2006M06</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2006M07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2006M08</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2006M09</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2006M10</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2006M11</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2006M12</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2007M01</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2007M02</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2007M03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2007M04</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2007M05</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2007M06</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2007M07</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2007M08</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2007M09</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2007M10</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2007M11</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2007M12</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2008M01</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2008M02</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2008M03</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2008M04</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2008M05</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2008M06</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2008M07</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2008M08</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2008M09</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2008M10</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2008M11</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2008M12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2009M01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2009M02</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2009M03</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2009M04</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2009M05</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2009M06</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2009M07</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2009M08</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2009M09</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2009M10</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2009M11</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2009M12</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2010M01</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2010M02</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2010M03</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2010M04</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2010M05</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2010M06</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2010M07</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2010M08</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2010M09</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2010M10</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2010M11</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2010M12</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2011M01</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2011M02</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2011M03</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2011M04</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2011M05</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2011M06</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2011M07</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2011M08</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2011M09</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2011M10</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2011M11</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2011M12</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2012M01</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2012M02</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2012M03</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2012M04</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2012M05</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2012M06</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2012M07</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2012M08</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2012M09</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2012M10</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2012M11</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2012M12</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2013M01</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2013M02</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2013M03</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2013M04</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2013M05</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2013M06</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2013M07</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2013M08</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2013M09</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2013M10</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2013M11</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2013M12</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2014M01</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2014M02</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2014M03</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2014M04</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2014M05</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2014M06</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2014M07</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2014M08</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2014M09</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2014M10</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2014M11</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2014M12</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2015M01</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2015M02</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2015M03</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2015M04</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2015M05</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2015M06</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2015M07</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2015M08</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2015M09</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2015M10</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2015M11</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2015M12</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2016M01</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2016M02</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2016M03</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2016M04</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2016M05</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2016M06</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2016M07</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2016M08</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2016M09</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2016M10</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2016M11</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2016M12</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2017M01</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2017M02</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2017M03</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2017M04</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2017M05</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2017M06</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2017M07</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2017M08</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2017M09</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2017M10</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2017M11</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2017M12</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2018M01</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2018M02</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2018M03</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2018M04</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2018M05</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2018M06</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2018M07</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>2018M08</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2018M09</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2018M10</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2018M11</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2018M12</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2019M01</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2019M02</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2019M03</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2019M04</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2019M05</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2019M06</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2019M07</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2019M08</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2019M09</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2019M10</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2019M11</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2019M12</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2020M01</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2020M02</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2020M03</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2020M04</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2020M05</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2020M06</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2020M07</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2020M08</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2020M09</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2020M10</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2020M11</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2020M12</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>2021M01</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2021M02</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2021M03</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2021M04</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>2021M05</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>2021M06</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>2021M07</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>2021M08</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>2021M09</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2021M10</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>2021M11</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>2021M12</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2022M01</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2022M02</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2022M03</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>2022M04</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>2022M05</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2022M06</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2022M07</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>2022M08</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>2022M09</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>2022M10</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>2022M11</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>2022M12</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>2023M01</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>2023M02</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>2023M03</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>2023M04</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>2023M05</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>2023M06</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>2023M07</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>2023M08</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>2023M09</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>2023M10</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>2023M11</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>2023M12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$277</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="276"/>
+                <c:pt idx="0">
+                  <c:v>5.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.63</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.93</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.03</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.47</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.34</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.17</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.29</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.96</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3.83</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>5.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C3E-4E2D-A113-B152F9CBF708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="495072840"/>
+        <c:axId val="495075792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="495072840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495075792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="495075792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495072840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E9BC658-2DE4-4361-BAF0-BDEC4917269C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1209,8 +3722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A2A376-17E5-47EC-81B1-588FF005095C}">
   <dimension ref="A1:B277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="A277" sqref="A277"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,7 +5658,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -3153,7 +5666,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3161,7 +5674,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -3169,7 +5682,7 @@
         <v>243</v>
       </c>
       <c r="B245">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -3177,7 +5690,7 @@
         <v>244</v>
       </c>
       <c r="B246">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3193,7 +5706,7 @@
         <v>246</v>
       </c>
       <c r="B248">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -3201,7 +5714,7 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3209,7 +5722,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -3217,7 +5730,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -3225,7 +5738,7 @@
         <v>250</v>
       </c>
       <c r="B252">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3233,7 +5746,7 @@
         <v>251</v>
       </c>
       <c r="B253">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -3257,7 +5770,7 @@
         <v>254</v>
       </c>
       <c r="B256">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -3273,7 +5786,7 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3281,7 +5794,7 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>1.21</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -3289,7 +5802,7 @@
         <v>258</v>
       </c>
       <c r="B260">
-        <v>1.68</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -3305,7 +5818,7 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>2.56</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -3321,7 +5834,7 @@
         <v>262</v>
       </c>
       <c r="B264">
-        <v>3.78</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -3329,7 +5842,7 @@
         <v>263</v>
       </c>
       <c r="B265">
-        <v>4.0999999999999996</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -3353,7 +5866,7 @@
         <v>266</v>
       </c>
       <c r="B268">
-        <v>4.6500000000000004</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -3369,7 +5882,7 @@
         <v>268</v>
       </c>
       <c r="B270">
-        <v>5.0599999999999996</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -3385,7 +5898,7 @@
         <v>270</v>
       </c>
       <c r="B272">
-        <v>5.12</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -3430,5 +5943,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>